<commit_message>
create function to create final order report
</commit_message>
<xml_diff>
--- a/orders/order_templates/10.09.2024.xlsx
+++ b/orders/order_templates/10.09.2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_work\_RTK\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{221B07CE-33A8-4F89-BEFC-71099D0EEDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E618898-20E0-4084-BAA2-7A7491C254FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="270" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,7 +366,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6368" uniqueCount="2737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6387" uniqueCount="2741">
   <si>
     <t>1.1.</t>
   </si>
@@ -8862,6 +8862,18 @@
   </si>
   <si>
     <t>03.12 Системы управления доступом к информационным ресурсам</t>
+  </si>
+  <si>
+    <t>Сотрудник 3</t>
+  </si>
+  <si>
+    <t>Парифный тлан</t>
+  </si>
+  <si>
+    <t>Продление</t>
+  </si>
+  <si>
+    <t>год</t>
   </si>
 </sst>
 </file>
@@ -10070,51 +10082,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="12" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="13" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="14" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="12" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="11" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="4" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="15" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="12" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="13" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="14" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -10150,6 +10117,51 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="12" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="13" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="14" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="4" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="15" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="7" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="12" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="13" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="14" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="17" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="11" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="18" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="12" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="13" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="14" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -10527,13 +10539,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="medium">
           <color indexed="64"/>
         </top>
@@ -10560,6 +10565,13 @@
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -10603,7 +10615,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D1DE854D-28B3-475A-9C81-FD620A605F27}" name="Таблица23" displayName="Таблица23" ref="A1:J280" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D1DE854D-28B3-475A-9C81-FD620A605F27}" name="Таблица23" displayName="Таблица23" ref="A1:J280" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A8C02378-4169-4B1B-B71C-F82B3506719B}" name="Наименование ПО" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{27150077-0FFB-4172-B6EC-358CE3F744A8}" name="Производитель ПО" dataDxfId="8"/>
@@ -10920,7 +10932,9 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:W449"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11175,9 +11189,7 @@
       <c r="N4" s="150">
         <v>200</v>
       </c>
-      <c r="O4" s="160">
-        <v>45910</v>
-      </c>
+      <c r="O4" s="160"/>
       <c r="P4" s="150" t="s">
         <v>185</v>
       </c>
@@ -11198,37 +11210,67 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A5" s="66"/>
-      <c r="B5" s="146"/>
-      <c r="C5" s="146"/>
-      <c r="D5" s="149"/>
-      <c r="E5" s="149"/>
-      <c r="F5" s="150"/>
+      <c r="A5" s="66">
+        <v>2</v>
+      </c>
+      <c r="B5" s="146">
+        <v>2024</v>
+      </c>
+      <c r="C5" s="146" t="s">
+        <v>2724</v>
+      </c>
+      <c r="D5" s="149" t="s">
+        <v>2448</v>
+      </c>
+      <c r="E5" s="149" t="s">
+        <v>2737</v>
+      </c>
+      <c r="F5" s="150" t="s">
+        <v>1843</v>
+      </c>
       <c r="G5" s="151" t="e">
         <f>VLOOKUP(F5,#REF!,2,)</f>
         <v>#REF!</v>
       </c>
-      <c r="H5" s="150"/>
-      <c r="I5" s="150"/>
+      <c r="H5" s="150" t="s">
+        <v>2738</v>
+      </c>
+      <c r="I5" s="150" t="s">
+        <v>2730</v>
+      </c>
       <c r="J5" s="151" t="e">
         <f>VLOOKUP(F5,#REF!,3,)</f>
         <v>#REF!</v>
       </c>
-      <c r="K5" s="150"/>
-      <c r="L5" s="150"/>
-      <c r="M5" s="150"/>
+      <c r="K5" s="150">
+        <v>1</v>
+      </c>
+      <c r="L5" s="150" t="s">
+        <v>2739</v>
+      </c>
+      <c r="M5" s="150">
+        <v>260</v>
+      </c>
       <c r="N5" s="150">
         <f>Заявки!$M5*Заявки!$K5</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="150"/>
-      <c r="P5" s="150"/>
-      <c r="Q5" s="150"/>
+        <v>260</v>
+      </c>
+      <c r="O5" s="160">
+        <v>45911</v>
+      </c>
+      <c r="P5" s="150" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q5" s="150" t="s">
+        <v>2740</v>
+      </c>
       <c r="R5" s="151" t="e">
         <f>VLOOKUP(F5,#REF!,6,)</f>
         <v>#REF!</v>
       </c>
-      <c r="S5" s="151"/>
+      <c r="S5" s="151" t="s">
+        <v>2205</v>
+      </c>
       <c r="T5" s="151" t="e">
         <f>VLOOKUP(F5,#REF!,4,)</f>
         <v>#REF!</v>
@@ -11239,37 +11281,63 @@
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A6" s="66"/>
-      <c r="B6" s="146"/>
-      <c r="C6" s="146"/>
-      <c r="D6" s="149"/>
-      <c r="E6" s="149"/>
-      <c r="F6" s="150"/>
+      <c r="A6" s="66">
+        <v>3</v>
+      </c>
+      <c r="B6" s="146">
+        <v>2024</v>
+      </c>
+      <c r="C6" s="146" t="s">
+        <v>2724</v>
+      </c>
+      <c r="D6" s="149" t="s">
+        <v>2446</v>
+      </c>
+      <c r="E6" s="149" t="s">
+        <v>2728</v>
+      </c>
+      <c r="F6" s="150" t="s">
+        <v>1849</v>
+      </c>
       <c r="G6" s="151" t="e">
         <f>VLOOKUP(F6,#REF!,2,)</f>
         <v>#REF!</v>
       </c>
-      <c r="H6" s="150"/>
+      <c r="H6" s="150" t="s">
+        <v>2738</v>
+      </c>
       <c r="I6" s="150"/>
       <c r="J6" s="151" t="e">
         <f>VLOOKUP(F6,#REF!,3,)</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="150"/>
-      <c r="L6" s="150"/>
-      <c r="M6" s="150"/>
+      <c r="K6" s="150">
+        <v>1</v>
+      </c>
+      <c r="L6" s="150" t="s">
+        <v>2731</v>
+      </c>
+      <c r="M6" s="150">
+        <v>5</v>
+      </c>
       <c r="N6" s="150">
         <f>Заявки!$M6*Заявки!$K6</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O6" s="150"/>
-      <c r="P6" s="150"/>
-      <c r="Q6" s="150"/>
+      <c r="P6" s="150" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q6" s="150" t="s">
+        <v>2740</v>
+      </c>
       <c r="R6" s="151" t="e">
         <f>VLOOKUP(F6,#REF!,6,)</f>
         <v>#REF!</v>
       </c>
-      <c r="S6" s="151"/>
+      <c r="S6" s="151" t="s">
+        <v>2263</v>
+      </c>
       <c r="T6" s="151" t="e">
         <f>VLOOKUP(F6,#REF!,4,)</f>
         <v>#REF!</v>
@@ -41503,39 +41571,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="170" t="s">
+      <c r="A1" s="176" t="s">
         <v>2463</v>
       </c>
-      <c r="B1" s="170" t="s">
+      <c r="B1" s="176" t="s">
         <v>2464</v>
       </c>
-      <c r="C1" s="170" t="s">
+      <c r="C1" s="176" t="s">
         <v>2465</v>
       </c>
-      <c r="D1" s="173" t="s">
+      <c r="D1" s="179" t="s">
         <v>2466</v>
       </c>
-      <c r="E1" s="174"/>
-      <c r="F1" s="174"/>
-      <c r="G1" s="175"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="181"/>
     </row>
     <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="171"/>
-      <c r="B2" s="171"/>
-      <c r="C2" s="171"/>
-      <c r="D2" s="173" t="s">
+      <c r="A2" s="177"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="179" t="s">
         <v>2467</v>
       </c>
-      <c r="E2" s="175"/>
-      <c r="F2" s="173" t="s">
+      <c r="E2" s="181"/>
+      <c r="F2" s="179" t="s">
         <v>2468</v>
       </c>
-      <c r="G2" s="175"/>
+      <c r="G2" s="181"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="172"/>
-      <c r="B3" s="172"/>
-      <c r="C3" s="172"/>
+      <c r="A3" s="178"/>
+      <c r="B3" s="178"/>
+      <c r="C3" s="178"/>
       <c r="D3" s="137" t="s">
         <v>2469</v>
       </c>
@@ -41550,15 +41618,15 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="161" t="s">
+      <c r="A4" s="173" t="s">
         <v>2471</v>
       </c>
-      <c r="B4" s="162"/>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="162"/>
-      <c r="G4" s="163"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="174"/>
+      <c r="D4" s="174"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="174"/>
+      <c r="G4" s="175"/>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="133" t="s">
@@ -41635,15 +41703,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="161" t="s">
+      <c r="A9" s="173" t="s">
         <v>2480</v>
       </c>
-      <c r="B9" s="162"/>
-      <c r="C9" s="162"/>
-      <c r="D9" s="162"/>
-      <c r="E9" s="162"/>
-      <c r="F9" s="162"/>
-      <c r="G9" s="163"/>
+      <c r="B9" s="174"/>
+      <c r="C9" s="174"/>
+      <c r="D9" s="174"/>
+      <c r="E9" s="174"/>
+      <c r="F9" s="174"/>
+      <c r="G9" s="175"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="133" t="s">
@@ -41655,12 +41723,12 @@
       <c r="C10" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D10" s="161" t="s">
+      <c r="D10" s="173" t="s">
         <v>2474</v>
       </c>
-      <c r="E10" s="162"/>
-      <c r="F10" s="162"/>
-      <c r="G10" s="163"/>
+      <c r="E10" s="174"/>
+      <c r="F10" s="174"/>
+      <c r="G10" s="175"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="136" t="s">
@@ -41672,12 +41740,12 @@
       <c r="C11" s="136" t="s">
         <v>2473</v>
       </c>
-      <c r="D11" s="167" t="s">
+      <c r="D11" s="182" t="s">
         <v>2476</v>
       </c>
-      <c r="E11" s="168"/>
-      <c r="F11" s="168"/>
-      <c r="G11" s="169"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="183"/>
+      <c r="G11" s="184"/>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="133" t="s">
@@ -41758,12 +41826,12 @@
       <c r="C15" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D15" s="161" t="s">
+      <c r="D15" s="173" t="s">
         <v>2489</v>
       </c>
-      <c r="E15" s="162"/>
-      <c r="F15" s="162"/>
-      <c r="G15" s="163"/>
+      <c r="E15" s="174"/>
+      <c r="F15" s="174"/>
+      <c r="G15" s="175"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="133" t="s">
@@ -41844,12 +41912,12 @@
       <c r="C19" s="136" t="s">
         <v>2473</v>
       </c>
-      <c r="D19" s="167" t="s">
+      <c r="D19" s="182" t="s">
         <v>2476</v>
       </c>
-      <c r="E19" s="168"/>
-      <c r="F19" s="168"/>
-      <c r="G19" s="169"/>
+      <c r="E19" s="183"/>
+      <c r="F19" s="183"/>
+      <c r="G19" s="184"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="133" t="s">
@@ -41861,12 +41929,12 @@
       <c r="C20" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D20" s="161" t="s">
+      <c r="D20" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E20" s="162"/>
-      <c r="F20" s="162"/>
-      <c r="G20" s="163"/>
+      <c r="E20" s="174"/>
+      <c r="F20" s="174"/>
+      <c r="G20" s="175"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="133" t="s">
@@ -41878,23 +41946,23 @@
       <c r="C21" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D21" s="161" t="s">
+      <c r="D21" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E21" s="162"/>
-      <c r="F21" s="162"/>
-      <c r="G21" s="163"/>
+      <c r="E21" s="174"/>
+      <c r="F21" s="174"/>
+      <c r="G21" s="175"/>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="161" t="s">
+      <c r="A22" s="173" t="s">
         <v>2497</v>
       </c>
-      <c r="B22" s="162"/>
-      <c r="C22" s="162"/>
-      <c r="D22" s="162"/>
-      <c r="E22" s="162"/>
-      <c r="F22" s="162"/>
-      <c r="G22" s="163"/>
+      <c r="B22" s="174"/>
+      <c r="C22" s="174"/>
+      <c r="D22" s="174"/>
+      <c r="E22" s="174"/>
+      <c r="F22" s="174"/>
+      <c r="G22" s="175"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="133" t="s">
@@ -41952,12 +42020,12 @@
       <c r="C25" s="136" t="s">
         <v>2473</v>
       </c>
-      <c r="D25" s="167" t="s">
+      <c r="D25" s="182" t="s">
         <v>2504</v>
       </c>
-      <c r="E25" s="168"/>
-      <c r="F25" s="168"/>
-      <c r="G25" s="169"/>
+      <c r="E25" s="183"/>
+      <c r="F25" s="183"/>
+      <c r="G25" s="184"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="133" t="s">
@@ -41992,12 +42060,12 @@
       <c r="C27" s="136" t="s">
         <v>2473</v>
       </c>
-      <c r="D27" s="167" t="s">
+      <c r="D27" s="182" t="s">
         <v>2476</v>
       </c>
-      <c r="E27" s="168"/>
-      <c r="F27" s="168"/>
-      <c r="G27" s="169"/>
+      <c r="E27" s="183"/>
+      <c r="F27" s="183"/>
+      <c r="G27" s="184"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="133" t="s">
@@ -42124,12 +42192,12 @@
       <c r="C33" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D33" s="161" t="s">
+      <c r="D33" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E33" s="162"/>
-      <c r="F33" s="162"/>
-      <c r="G33" s="163"/>
+      <c r="E33" s="174"/>
+      <c r="F33" s="174"/>
+      <c r="G33" s="175"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="133" t="s">
@@ -42187,12 +42255,12 @@
       <c r="C36" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D36" s="161" t="s">
+      <c r="D36" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E36" s="162"/>
-      <c r="F36" s="162"/>
-      <c r="G36" s="163"/>
+      <c r="E36" s="174"/>
+      <c r="F36" s="174"/>
+      <c r="G36" s="175"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="133" t="s">
@@ -42227,12 +42295,12 @@
       <c r="C38" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D38" s="161" t="s">
+      <c r="D38" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E38" s="162"/>
-      <c r="F38" s="162"/>
-      <c r="G38" s="163"/>
+      <c r="E38" s="174"/>
+      <c r="F38" s="174"/>
+      <c r="G38" s="175"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="133" t="s">
@@ -42258,15 +42326,15 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="161" t="s">
+      <c r="A40" s="173" t="s">
         <v>2534</v>
       </c>
-      <c r="B40" s="162"/>
-      <c r="C40" s="162"/>
-      <c r="D40" s="162"/>
-      <c r="E40" s="162"/>
-      <c r="F40" s="162"/>
-      <c r="G40" s="163"/>
+      <c r="B40" s="174"/>
+      <c r="C40" s="174"/>
+      <c r="D40" s="174"/>
+      <c r="E40" s="174"/>
+      <c r="F40" s="174"/>
+      <c r="G40" s="175"/>
     </row>
     <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="133" t="s">
@@ -42278,12 +42346,12 @@
       <c r="C41" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D41" s="161" t="s">
+      <c r="D41" s="173" t="s">
         <v>2537</v>
       </c>
-      <c r="E41" s="162"/>
-      <c r="F41" s="162"/>
-      <c r="G41" s="163"/>
+      <c r="E41" s="174"/>
+      <c r="F41" s="174"/>
+      <c r="G41" s="175"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="133" t="s">
@@ -42387,10 +42455,10 @@
       <c r="C46" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="161" t="s">
+      <c r="D46" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E46" s="163"/>
+      <c r="E46" s="175"/>
       <c r="F46" s="132" t="s">
         <v>2473</v>
       </c>
@@ -42408,12 +42476,12 @@
       <c r="C47" s="135" t="s">
         <v>2473</v>
       </c>
-      <c r="D47" s="161" t="s">
+      <c r="D47" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E47" s="162"/>
-      <c r="F47" s="162"/>
-      <c r="G47" s="163"/>
+      <c r="E47" s="174"/>
+      <c r="F47" s="174"/>
+      <c r="G47" s="175"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="133" t="s">
@@ -42448,23 +42516,23 @@
       <c r="C49" s="135" t="s">
         <v>2473</v>
       </c>
-      <c r="D49" s="161" t="s">
+      <c r="D49" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E49" s="162"/>
-      <c r="F49" s="162"/>
-      <c r="G49" s="163"/>
+      <c r="E49" s="174"/>
+      <c r="F49" s="174"/>
+      <c r="G49" s="175"/>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="164" t="s">
+      <c r="A50" s="185" t="s">
         <v>2555</v>
       </c>
-      <c r="B50" s="165"/>
-      <c r="C50" s="165"/>
-      <c r="D50" s="165"/>
-      <c r="E50" s="165"/>
-      <c r="F50" s="165"/>
-      <c r="G50" s="166"/>
+      <c r="B50" s="186"/>
+      <c r="C50" s="186"/>
+      <c r="D50" s="186"/>
+      <c r="E50" s="186"/>
+      <c r="F50" s="186"/>
+      <c r="G50" s="187"/>
     </row>
     <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="133" t="s">
@@ -42499,12 +42567,12 @@
       <c r="C52" s="135" t="s">
         <v>2473</v>
       </c>
-      <c r="D52" s="161" t="s">
+      <c r="D52" s="173" t="s">
         <v>2560</v>
       </c>
-      <c r="E52" s="162"/>
-      <c r="F52" s="162"/>
-      <c r="G52" s="163"/>
+      <c r="E52" s="174"/>
+      <c r="F52" s="174"/>
+      <c r="G52" s="175"/>
     </row>
     <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="133" t="s">
@@ -42539,12 +42607,12 @@
       <c r="C54" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D54" s="161" t="s">
+      <c r="D54" s="173" t="s">
         <v>2560</v>
       </c>
-      <c r="E54" s="162"/>
-      <c r="F54" s="162"/>
-      <c r="G54" s="163"/>
+      <c r="E54" s="174"/>
+      <c r="F54" s="174"/>
+      <c r="G54" s="175"/>
     </row>
     <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="133" t="s">
@@ -42602,12 +42670,12 @@
       <c r="C57" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D57" s="161" t="s">
+      <c r="D57" s="173" t="s">
         <v>2572</v>
       </c>
-      <c r="E57" s="162"/>
-      <c r="F57" s="162"/>
-      <c r="G57" s="163"/>
+      <c r="E57" s="174"/>
+      <c r="F57" s="174"/>
+      <c r="G57" s="175"/>
     </row>
     <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="133" t="s">
@@ -42688,12 +42756,12 @@
       <c r="C61" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D61" s="161" t="s">
+      <c r="D61" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E61" s="162"/>
-      <c r="F61" s="162"/>
-      <c r="G61" s="163"/>
+      <c r="E61" s="174"/>
+      <c r="F61" s="174"/>
+      <c r="G61" s="175"/>
     </row>
     <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="133" t="s">
@@ -42705,12 +42773,12 @@
       <c r="C62" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D62" s="161" t="s">
+      <c r="D62" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E62" s="162"/>
-      <c r="F62" s="162"/>
-      <c r="G62" s="163"/>
+      <c r="E62" s="174"/>
+      <c r="F62" s="174"/>
+      <c r="G62" s="175"/>
     </row>
     <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="133" t="s">
@@ -42722,12 +42790,12 @@
       <c r="C63" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D63" s="161" t="s">
+      <c r="D63" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E63" s="162"/>
-      <c r="F63" s="162"/>
-      <c r="G63" s="163"/>
+      <c r="E63" s="174"/>
+      <c r="F63" s="174"/>
+      <c r="G63" s="175"/>
     </row>
     <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="133" t="s">
@@ -42785,23 +42853,23 @@
       <c r="C66" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D66" s="161" t="s">
+      <c r="D66" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E66" s="162"/>
-      <c r="F66" s="162"/>
-      <c r="G66" s="163"/>
+      <c r="E66" s="174"/>
+      <c r="F66" s="174"/>
+      <c r="G66" s="175"/>
     </row>
     <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="161" t="s">
+      <c r="A67" s="173" t="s">
         <v>2593</v>
       </c>
-      <c r="B67" s="162"/>
-      <c r="C67" s="162"/>
-      <c r="D67" s="162"/>
-      <c r="E67" s="162"/>
-      <c r="F67" s="162"/>
-      <c r="G67" s="163"/>
+      <c r="B67" s="174"/>
+      <c r="C67" s="174"/>
+      <c r="D67" s="174"/>
+      <c r="E67" s="174"/>
+      <c r="F67" s="174"/>
+      <c r="G67" s="175"/>
     </row>
     <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="133" t="s">
@@ -42905,12 +42973,12 @@
       <c r="C72" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D72" s="161" t="s">
+      <c r="D72" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E72" s="162"/>
-      <c r="F72" s="162"/>
-      <c r="G72" s="163"/>
+      <c r="E72" s="174"/>
+      <c r="F72" s="174"/>
+      <c r="G72" s="175"/>
     </row>
     <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="133" t="s">
@@ -42922,12 +42990,12 @@
       <c r="C73" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D73" s="161" t="s">
+      <c r="D73" s="173" t="s">
         <v>2607</v>
       </c>
-      <c r="E73" s="162"/>
-      <c r="F73" s="162"/>
-      <c r="G73" s="163"/>
+      <c r="E73" s="174"/>
+      <c r="F73" s="174"/>
+      <c r="G73" s="175"/>
     </row>
     <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="133" t="s">
@@ -42985,12 +43053,12 @@
       <c r="C76" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D76" s="161" t="s">
+      <c r="D76" s="173" t="s">
         <v>2607</v>
       </c>
-      <c r="E76" s="162"/>
-      <c r="F76" s="162"/>
-      <c r="G76" s="163"/>
+      <c r="E76" s="174"/>
+      <c r="F76" s="174"/>
+      <c r="G76" s="175"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="133" t="s">
@@ -43002,12 +43070,12 @@
       <c r="C77" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D77" s="161" t="s">
+      <c r="D77" s="173" t="s">
         <v>2607</v>
       </c>
-      <c r="E77" s="162"/>
-      <c r="F77" s="162"/>
-      <c r="G77" s="163"/>
+      <c r="E77" s="174"/>
+      <c r="F77" s="174"/>
+      <c r="G77" s="175"/>
     </row>
     <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="133" t="s">
@@ -43019,12 +43087,12 @@
       <c r="C78" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D78" s="161" t="s">
+      <c r="D78" s="173" t="s">
         <v>2607</v>
       </c>
-      <c r="E78" s="162"/>
-      <c r="F78" s="162"/>
-      <c r="G78" s="163"/>
+      <c r="E78" s="174"/>
+      <c r="F78" s="174"/>
+      <c r="G78" s="175"/>
     </row>
     <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="133" t="s">
@@ -43050,15 +43118,15 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="161" t="s">
+      <c r="A80" s="173" t="s">
         <v>2620</v>
       </c>
-      <c r="B80" s="162"/>
-      <c r="C80" s="162"/>
-      <c r="D80" s="162"/>
-      <c r="E80" s="162"/>
-      <c r="F80" s="162"/>
-      <c r="G80" s="163"/>
+      <c r="B80" s="174"/>
+      <c r="C80" s="174"/>
+      <c r="D80" s="174"/>
+      <c r="E80" s="174"/>
+      <c r="F80" s="174"/>
+      <c r="G80" s="175"/>
     </row>
     <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="133" t="s">
@@ -43070,12 +43138,12 @@
       <c r="C81" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D81" s="161" t="s">
+      <c r="D81" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E81" s="162"/>
-      <c r="F81" s="162"/>
-      <c r="G81" s="163"/>
+      <c r="E81" s="174"/>
+      <c r="F81" s="174"/>
+      <c r="G81" s="175"/>
     </row>
     <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="133" t="s">
@@ -43087,12 +43155,12 @@
       <c r="C82" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D82" s="161" t="s">
+      <c r="D82" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E82" s="162"/>
-      <c r="F82" s="162"/>
-      <c r="G82" s="163"/>
+      <c r="E82" s="174"/>
+      <c r="F82" s="174"/>
+      <c r="G82" s="175"/>
     </row>
     <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="133" t="s">
@@ -43150,12 +43218,12 @@
       <c r="C85" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D85" s="161" t="s">
+      <c r="D85" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E85" s="162"/>
-      <c r="F85" s="162"/>
-      <c r="G85" s="163"/>
+      <c r="E85" s="174"/>
+      <c r="F85" s="174"/>
+      <c r="G85" s="175"/>
     </row>
     <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="133" t="s">
@@ -43167,12 +43235,12 @@
       <c r="C86" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D86" s="161" t="s">
+      <c r="D86" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E86" s="162"/>
-      <c r="F86" s="162"/>
-      <c r="G86" s="163"/>
+      <c r="E86" s="174"/>
+      <c r="F86" s="174"/>
+      <c r="G86" s="175"/>
     </row>
     <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="133" t="s">
@@ -43184,23 +43252,23 @@
       <c r="C87" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D87" s="161" t="s">
+      <c r="D87" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E87" s="162"/>
-      <c r="F87" s="162"/>
-      <c r="G87" s="163"/>
+      <c r="E87" s="174"/>
+      <c r="F87" s="174"/>
+      <c r="G87" s="175"/>
     </row>
     <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="161" t="s">
+      <c r="A88" s="173" t="s">
         <v>2636</v>
       </c>
-      <c r="B88" s="162"/>
-      <c r="C88" s="162"/>
-      <c r="D88" s="162"/>
-      <c r="E88" s="162"/>
-      <c r="F88" s="162"/>
-      <c r="G88" s="163"/>
+      <c r="B88" s="174"/>
+      <c r="C88" s="174"/>
+      <c r="D88" s="174"/>
+      <c r="E88" s="174"/>
+      <c r="F88" s="174"/>
+      <c r="G88" s="175"/>
     </row>
     <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="133" t="s">
@@ -43212,12 +43280,12 @@
       <c r="C89" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D89" s="161" t="s">
+      <c r="D89" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E89" s="162"/>
-      <c r="F89" s="162"/>
-      <c r="G89" s="163"/>
+      <c r="E89" s="174"/>
+      <c r="F89" s="174"/>
+      <c r="G89" s="175"/>
     </row>
     <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A90" s="133" t="s">
@@ -43229,12 +43297,12 @@
       <c r="C90" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D90" s="161" t="s">
+      <c r="D90" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E90" s="162"/>
-      <c r="F90" s="162"/>
-      <c r="G90" s="163"/>
+      <c r="E90" s="174"/>
+      <c r="F90" s="174"/>
+      <c r="G90" s="175"/>
     </row>
     <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A91" s="133" t="s">
@@ -43269,12 +43337,12 @@
       <c r="C92" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D92" s="161" t="s">
+      <c r="D92" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E92" s="162"/>
-      <c r="F92" s="162"/>
-      <c r="G92" s="163"/>
+      <c r="E92" s="174"/>
+      <c r="F92" s="174"/>
+      <c r="G92" s="175"/>
     </row>
     <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A93" s="133" t="s">
@@ -43286,12 +43354,12 @@
       <c r="C93" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D93" s="161" t="s">
+      <c r="D93" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E93" s="162"/>
-      <c r="F93" s="162"/>
-      <c r="G93" s="163"/>
+      <c r="E93" s="174"/>
+      <c r="F93" s="174"/>
+      <c r="G93" s="175"/>
     </row>
     <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="133" t="s">
@@ -43303,12 +43371,12 @@
       <c r="C94" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D94" s="161" t="s">
+      <c r="D94" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E94" s="162"/>
-      <c r="F94" s="162"/>
-      <c r="G94" s="163"/>
+      <c r="E94" s="174"/>
+      <c r="F94" s="174"/>
+      <c r="G94" s="175"/>
     </row>
     <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="133" t="s">
@@ -43320,12 +43388,12 @@
       <c r="C95" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D95" s="161" t="s">
+      <c r="D95" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E95" s="162"/>
-      <c r="F95" s="162"/>
-      <c r="G95" s="163"/>
+      <c r="E95" s="174"/>
+      <c r="F95" s="174"/>
+      <c r="G95" s="175"/>
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="133" t="s">
@@ -43337,12 +43405,12 @@
       <c r="C96" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D96" s="161" t="s">
+      <c r="D96" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E96" s="162"/>
-      <c r="F96" s="162"/>
-      <c r="G96" s="163"/>
+      <c r="E96" s="174"/>
+      <c r="F96" s="174"/>
+      <c r="G96" s="175"/>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="133" t="s">
@@ -43354,12 +43422,12 @@
       <c r="C97" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D97" s="161" t="s">
+      <c r="D97" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E97" s="162"/>
-      <c r="F97" s="162"/>
-      <c r="G97" s="163"/>
+      <c r="E97" s="174"/>
+      <c r="F97" s="174"/>
+      <c r="G97" s="175"/>
     </row>
     <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="133" t="s">
@@ -43371,12 +43439,12 @@
       <c r="C98" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D98" s="161" t="s">
+      <c r="D98" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E98" s="162"/>
-      <c r="F98" s="162"/>
-      <c r="G98" s="163"/>
+      <c r="E98" s="174"/>
+      <c r="F98" s="174"/>
+      <c r="G98" s="175"/>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="133" t="s">
@@ -43388,23 +43456,23 @@
       <c r="C99" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D99" s="161" t="s">
+      <c r="D99" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E99" s="162"/>
-      <c r="F99" s="162"/>
-      <c r="G99" s="163"/>
+      <c r="E99" s="174"/>
+      <c r="F99" s="174"/>
+      <c r="G99" s="175"/>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="161" t="s">
+      <c r="A100" s="173" t="s">
         <v>2660</v>
       </c>
-      <c r="B100" s="162"/>
-      <c r="C100" s="162"/>
-      <c r="D100" s="162"/>
-      <c r="E100" s="162"/>
-      <c r="F100" s="162"/>
-      <c r="G100" s="163"/>
+      <c r="B100" s="174"/>
+      <c r="C100" s="174"/>
+      <c r="D100" s="174"/>
+      <c r="E100" s="174"/>
+      <c r="F100" s="174"/>
+      <c r="G100" s="175"/>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="133" t="s">
@@ -43439,12 +43507,12 @@
       <c r="C102" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D102" s="161" t="s">
+      <c r="D102" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E102" s="162"/>
-      <c r="F102" s="162"/>
-      <c r="G102" s="163"/>
+      <c r="E102" s="174"/>
+      <c r="F102" s="174"/>
+      <c r="G102" s="175"/>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="133" t="s">
@@ -43456,12 +43524,12 @@
       <c r="C103" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D103" s="161" t="s">
+      <c r="D103" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E103" s="162"/>
-      <c r="F103" s="162"/>
-      <c r="G103" s="163"/>
+      <c r="E103" s="174"/>
+      <c r="F103" s="174"/>
+      <c r="G103" s="175"/>
     </row>
     <row r="104" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A104" s="133" t="s">
@@ -43473,12 +43541,12 @@
       <c r="C104" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D104" s="161" t="s">
+      <c r="D104" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E104" s="162"/>
-      <c r="F104" s="162"/>
-      <c r="G104" s="163"/>
+      <c r="E104" s="174"/>
+      <c r="F104" s="174"/>
+      <c r="G104" s="175"/>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A105" s="133" t="s">
@@ -43513,12 +43581,12 @@
       <c r="C106" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D106" s="161" t="s">
+      <c r="D106" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E106" s="162"/>
-      <c r="F106" s="162"/>
-      <c r="G106" s="163"/>
+      <c r="E106" s="174"/>
+      <c r="F106" s="174"/>
+      <c r="G106" s="175"/>
     </row>
     <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A107" s="133" t="s">
@@ -43622,12 +43690,12 @@
       <c r="C111" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D111" s="161" t="s">
+      <c r="D111" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E111" s="162"/>
-      <c r="F111" s="162"/>
-      <c r="G111" s="163"/>
+      <c r="E111" s="174"/>
+      <c r="F111" s="174"/>
+      <c r="G111" s="175"/>
     </row>
     <row r="112" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A112" s="133" t="s">
@@ -43676,15 +43744,15 @@
       </c>
     </row>
     <row r="114" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="161" t="s">
+      <c r="A114" s="173" t="s">
         <v>2691</v>
       </c>
-      <c r="B114" s="162"/>
-      <c r="C114" s="162"/>
-      <c r="D114" s="162"/>
-      <c r="E114" s="162"/>
-      <c r="F114" s="162"/>
-      <c r="G114" s="163"/>
+      <c r="B114" s="174"/>
+      <c r="C114" s="174"/>
+      <c r="D114" s="174"/>
+      <c r="E114" s="174"/>
+      <c r="F114" s="174"/>
+      <c r="G114" s="175"/>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="133" t="s">
@@ -43719,12 +43787,12 @@
       <c r="C116" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D116" s="161" t="s">
+      <c r="D116" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E116" s="162"/>
-      <c r="F116" s="162"/>
-      <c r="G116" s="163"/>
+      <c r="E116" s="174"/>
+      <c r="F116" s="174"/>
+      <c r="G116" s="175"/>
     </row>
     <row r="117" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A117" s="133" t="s">
@@ -43736,12 +43804,12 @@
       <c r="C117" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D117" s="161" t="s">
+      <c r="D117" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E117" s="162"/>
-      <c r="F117" s="162"/>
-      <c r="G117" s="163"/>
+      <c r="E117" s="174"/>
+      <c r="F117" s="174"/>
+      <c r="G117" s="175"/>
     </row>
     <row r="118" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="133" t="s">
@@ -43767,15 +43835,15 @@
       </c>
     </row>
     <row r="119" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="161" t="s">
+      <c r="A119" s="173" t="s">
         <v>2702</v>
       </c>
-      <c r="B119" s="162"/>
-      <c r="C119" s="162"/>
-      <c r="D119" s="162"/>
-      <c r="E119" s="162"/>
-      <c r="F119" s="162"/>
-      <c r="G119" s="163"/>
+      <c r="B119" s="174"/>
+      <c r="C119" s="174"/>
+      <c r="D119" s="174"/>
+      <c r="E119" s="174"/>
+      <c r="F119" s="174"/>
+      <c r="G119" s="175"/>
     </row>
     <row r="120" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="133" t="s">
@@ -43810,12 +43878,12 @@
       <c r="C121" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D121" s="161" t="s">
+      <c r="D121" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E121" s="162"/>
-      <c r="F121" s="162"/>
-      <c r="G121" s="163"/>
+      <c r="E121" s="174"/>
+      <c r="F121" s="174"/>
+      <c r="G121" s="175"/>
     </row>
     <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="133" t="s">
@@ -43850,12 +43918,12 @@
       <c r="C123" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D123" s="161" t="s">
+      <c r="D123" s="173" t="s">
         <v>2476</v>
       </c>
-      <c r="E123" s="162"/>
-      <c r="F123" s="162"/>
-      <c r="G123" s="163"/>
+      <c r="E123" s="174"/>
+      <c r="F123" s="174"/>
+      <c r="G123" s="175"/>
     </row>
     <row r="124" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="133" t="s">
@@ -43890,23 +43958,62 @@
       <c r="C125" s="132" t="s">
         <v>2473</v>
       </c>
-      <c r="D125" s="161" t="s">
+      <c r="D125" s="173" t="s">
         <v>2717</v>
       </c>
-      <c r="E125" s="162"/>
-      <c r="F125" s="162"/>
-      <c r="G125" s="163"/>
+      <c r="E125" s="174"/>
+      <c r="F125" s="174"/>
+      <c r="G125" s="175"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:G3" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="69">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D123:G123"/>
+    <mergeCell ref="D125:G125"/>
+    <mergeCell ref="D106:G106"/>
+    <mergeCell ref="D111:G111"/>
+    <mergeCell ref="A114:G114"/>
+    <mergeCell ref="D116:G116"/>
+    <mergeCell ref="D117:G117"/>
+    <mergeCell ref="A119:G119"/>
+    <mergeCell ref="D99:G99"/>
+    <mergeCell ref="A100:G100"/>
+    <mergeCell ref="D90:G90"/>
+    <mergeCell ref="D103:G103"/>
+    <mergeCell ref="D121:G121"/>
+    <mergeCell ref="D104:G104"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="D102:G102"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="D87:G87"/>
+    <mergeCell ref="A88:G88"/>
+    <mergeCell ref="D89:G89"/>
+    <mergeCell ref="D92:G92"/>
+    <mergeCell ref="D93:G93"/>
+    <mergeCell ref="D94:G94"/>
+    <mergeCell ref="D95:G95"/>
+    <mergeCell ref="D96:G96"/>
+    <mergeCell ref="D97:G97"/>
+    <mergeCell ref="D98:G98"/>
+    <mergeCell ref="D82:G82"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="D76:G76"/>
+    <mergeCell ref="D77:G77"/>
     <mergeCell ref="A9:G9"/>
     <mergeCell ref="D47:G47"/>
     <mergeCell ref="D27:G27"/>
@@ -43923,52 +44030,13 @@
     <mergeCell ref="D36:G36"/>
     <mergeCell ref="D38:G38"/>
     <mergeCell ref="A40:G40"/>
-    <mergeCell ref="D82:G82"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="D57:G57"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="D63:G63"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="A67:G67"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="D76:G76"/>
-    <mergeCell ref="D77:G77"/>
-    <mergeCell ref="D78:G78"/>
-    <mergeCell ref="A80:G80"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="D102:G102"/>
-    <mergeCell ref="D85:G85"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="D87:G87"/>
-    <mergeCell ref="A88:G88"/>
-    <mergeCell ref="D89:G89"/>
-    <mergeCell ref="D92:G92"/>
-    <mergeCell ref="D93:G93"/>
-    <mergeCell ref="D94:G94"/>
-    <mergeCell ref="D95:G95"/>
-    <mergeCell ref="D96:G96"/>
-    <mergeCell ref="D97:G97"/>
-    <mergeCell ref="D98:G98"/>
-    <mergeCell ref="D99:G99"/>
-    <mergeCell ref="A100:G100"/>
-    <mergeCell ref="D90:G90"/>
-    <mergeCell ref="D103:G103"/>
-    <mergeCell ref="D121:G121"/>
-    <mergeCell ref="D123:G123"/>
-    <mergeCell ref="D125:G125"/>
-    <mergeCell ref="D106:G106"/>
-    <mergeCell ref="D111:G111"/>
-    <mergeCell ref="A114:G114"/>
-    <mergeCell ref="D116:G116"/>
-    <mergeCell ref="D117:G117"/>
-    <mergeCell ref="A119:G119"/>
-    <mergeCell ref="D104:G104"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -43989,7 +44057,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="161" t="s">
         <v>2733</v>
       </c>
     </row>
@@ -44399,7 +44467,7 @@
       <c r="G10" s="80" t="s">
         <v>234</v>
       </c>
-      <c r="H10" s="177" t="s">
+      <c r="H10" s="162" t="s">
         <v>235</v>
       </c>
       <c r="I10" s="84" t="s">
@@ -44739,7 +44807,7 @@
       <c r="Z18" s="75"/>
     </row>
     <row r="19" spans="1:26" s="121" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="178" t="s">
+      <c r="A19" s="163" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="52" t="s">
@@ -44859,7 +44927,7 @@
       <c r="M22" s="116"/>
     </row>
     <row r="23" spans="1:26" s="121" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="179" t="s">
+      <c r="A23" s="164" t="s">
         <v>117</v>
       </c>
       <c r="B23" s="52" t="s">
@@ -45072,7 +45140,7 @@
         <v>2129</v>
       </c>
       <c r="G29" s="80"/>
-      <c r="H29" s="177"/>
+      <c r="H29" s="162"/>
       <c r="I29" s="84" t="s">
         <v>283</v>
       </c>
@@ -45113,7 +45181,7 @@
       <c r="M30" s="116"/>
     </row>
     <row r="31" spans="1:26" s="121" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="178" t="s">
+      <c r="A31" s="163" t="s">
         <v>116</v>
       </c>
       <c r="B31" s="52" t="s">
@@ -45175,7 +45243,7 @@
       <c r="M32" s="116"/>
     </row>
     <row r="33" spans="1:26" s="121" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="178" t="s">
+      <c r="A33" s="163" t="s">
         <v>1869</v>
       </c>
       <c r="B33" s="52" t="s">
@@ -45250,7 +45318,7 @@
       <c r="Z34" s="75"/>
     </row>
     <row r="35" spans="1:26" s="121" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="179" t="s">
+      <c r="A35" s="164" t="s">
         <v>1874</v>
       </c>
       <c r="B35" s="52" t="s">
@@ -45350,7 +45418,7 @@
       <c r="G37" s="80" t="s">
         <v>297</v>
       </c>
-      <c r="H37" s="177"/>
+      <c r="H37" s="162"/>
       <c r="I37" s="84" t="s">
         <v>283</v>
       </c>
@@ -45613,7 +45681,7 @@
       <c r="Z43" s="75"/>
     </row>
     <row r="44" spans="1:26" s="121" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="178" t="s">
+      <c r="A44" s="163" t="s">
         <v>56</v>
       </c>
       <c r="B44" s="52" t="s">
@@ -45644,7 +45712,7 @@
       <c r="M44" s="116"/>
     </row>
     <row r="45" spans="1:26" s="121" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="179" t="s">
+      <c r="A45" s="164" t="s">
         <v>1897</v>
       </c>
       <c r="B45" s="52" t="s">
@@ -46064,7 +46132,7 @@
       <c r="G56" s="80" t="s">
         <v>300</v>
       </c>
-      <c r="H56" s="177" t="s">
+      <c r="H56" s="162" t="s">
         <v>301</v>
       </c>
       <c r="I56" s="84" t="s">
@@ -46170,7 +46238,7 @@
       <c r="G59" s="80" t="s">
         <v>294</v>
       </c>
-      <c r="H59" s="177" t="s">
+      <c r="H59" s="162" t="s">
         <v>262</v>
       </c>
       <c r="I59" s="84" t="s">
@@ -46328,7 +46396,7 @@
       <c r="M63" s="75"/>
     </row>
     <row r="64" spans="1:26" s="121" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="178" t="s">
+      <c r="A64" s="163" t="s">
         <v>367</v>
       </c>
       <c r="B64" s="52" t="s">
@@ -46659,7 +46727,7 @@
       <c r="M72" s="75"/>
     </row>
     <row r="73" spans="1:26" s="121" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="178" t="s">
+      <c r="A73" s="163" t="s">
         <v>1942</v>
       </c>
       <c r="B73" s="52"/>
@@ -47044,7 +47112,7 @@
       <c r="G83" s="82" t="s">
         <v>323</v>
       </c>
-      <c r="H83" s="180" t="s">
+      <c r="H83" s="165" t="s">
         <v>319</v>
       </c>
       <c r="I83" s="84" t="s">
@@ -47790,7 +47858,7 @@
       <c r="Z100" s="121"/>
     </row>
     <row r="101" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A101" s="181" t="s">
+      <c r="A101" s="166" t="s">
         <v>1983</v>
       </c>
       <c r="B101" s="83" t="s">
@@ -47852,7 +47920,7 @@
       <c r="G102" s="80" t="s">
         <v>248</v>
       </c>
-      <c r="H102" s="177" t="s">
+      <c r="H102" s="162" t="s">
         <v>249</v>
       </c>
       <c r="I102" s="84" t="s">
@@ -48199,7 +48267,7 @@
         <v>2132</v>
       </c>
       <c r="G111" s="80"/>
-      <c r="H111" s="177"/>
+      <c r="H111" s="162"/>
       <c r="I111" s="84" t="s">
         <v>283</v>
       </c>
@@ -48343,7 +48411,7 @@
       <c r="G115" s="80" t="s">
         <v>294</v>
       </c>
-      <c r="H115" s="177"/>
+      <c r="H115" s="162"/>
       <c r="I115" s="84" t="s">
         <v>1842</v>
       </c>
@@ -48461,7 +48529,7 @@
       <c r="G118" s="80" t="s">
         <v>294</v>
       </c>
-      <c r="H118" s="177" t="s">
+      <c r="H118" s="162" t="s">
         <v>397</v>
       </c>
       <c r="I118" s="84" t="s">
@@ -48486,7 +48554,7 @@
       <c r="Z118" s="121"/>
     </row>
     <row r="119" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A119" s="178" t="s">
+      <c r="A119" s="163" t="s">
         <v>2111</v>
       </c>
       <c r="B119" s="52" t="s">
@@ -48618,7 +48686,7 @@
       <c r="Z121" s="121"/>
     </row>
     <row r="122" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A122" s="182" t="s">
+      <c r="A122" s="167" t="s">
         <v>100</v>
       </c>
       <c r="B122" s="83" t="s">
@@ -49221,7 +49289,7 @@
       <c r="J137" s="77"/>
     </row>
     <row r="138" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A138" s="178" t="s">
+      <c r="A138" s="163" t="s">
         <v>2047</v>
       </c>
       <c r="B138" s="52" t="s">
@@ -49261,7 +49329,7 @@
       <c r="Z138" s="121"/>
     </row>
     <row r="139" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A139" s="178" t="s">
+      <c r="A139" s="163" t="s">
         <v>114</v>
       </c>
       <c r="B139" s="52" t="s">
@@ -49376,7 +49444,7 @@
       <c r="Z141" s="121"/>
     </row>
     <row r="142" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A142" s="179" t="s">
+      <c r="A142" s="164" t="s">
         <v>75</v>
       </c>
       <c r="B142" s="52" t="s">
@@ -49568,7 +49636,7 @@
       </c>
     </row>
     <row r="147" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A147" s="178" t="s">
+      <c r="A147" s="163" t="s">
         <v>2056</v>
       </c>
       <c r="B147" s="52" t="s">
@@ -49794,7 +49862,7 @@
       <c r="J152" s="77"/>
     </row>
     <row r="153" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A153" s="183" t="s">
+      <c r="A153" s="168" t="s">
         <v>105</v>
       </c>
       <c r="B153" s="83" t="s">
@@ -49969,7 +50037,7 @@
         <v>2135</v>
       </c>
       <c r="G157" s="80"/>
-      <c r="H157" s="177"/>
+      <c r="H157" s="162"/>
       <c r="I157" s="84" t="s">
         <v>283</v>
       </c>
@@ -50250,7 +50318,7 @@
       <c r="G164" s="80" t="s">
         <v>294</v>
       </c>
-      <c r="H164" s="177"/>
+      <c r="H164" s="162"/>
       <c r="I164" s="84" t="s">
         <v>1842</v>
       </c>
@@ -50499,7 +50567,7 @@
       <c r="Z170" s="121"/>
     </row>
     <row r="171" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A171" s="184" t="s">
+      <c r="A171" s="169" t="s">
         <v>2089</v>
       </c>
       <c r="B171" s="83"/>
@@ -50554,7 +50622,7 @@
       <c r="G172" s="80" t="s">
         <v>283</v>
       </c>
-      <c r="H172" s="185" t="s">
+      <c r="H172" s="170" t="s">
         <v>2092</v>
       </c>
       <c r="I172" s="84" t="s">
@@ -50578,7 +50646,7 @@
       <c r="Z172" s="121"/>
     </row>
     <row r="173" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A173" s="178" t="s">
+      <c r="A173" s="163" t="s">
         <v>2093</v>
       </c>
       <c r="B173" s="65" t="s">
@@ -52304,26 +52372,26 @@
       <c r="M243" s="124"/>
     </row>
     <row r="244" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A244" s="186" t="s">
+      <c r="A244" s="171" t="s">
         <v>2369</v>
       </c>
-      <c r="B244" s="187" t="s">
+      <c r="B244" s="172" t="s">
         <v>2368</v>
       </c>
-      <c r="C244" s="186" t="s">
+      <c r="C244" s="171" t="s">
         <v>139</v>
       </c>
-      <c r="D244" s="186"/>
-      <c r="E244" s="186"/>
-      <c r="F244" s="186" t="s">
+      <c r="D244" s="171"/>
+      <c r="E244" s="171"/>
+      <c r="F244" s="171" t="s">
         <v>2269</v>
       </c>
-      <c r="G244" s="186"/>
-      <c r="H244" s="186"/>
-      <c r="I244" s="186" t="s">
+      <c r="G244" s="171"/>
+      <c r="H244" s="171"/>
+      <c r="I244" s="171" t="s">
         <v>1842</v>
       </c>
-      <c r="J244" s="186">
+      <c r="J244" s="171">
         <v>1217</v>
       </c>
       <c r="K244" s="129"/>

</xml_diff>

<commit_message>
finished treeview; fixed grouping logic; added progress bar and errors for loading files; implemented refresh button; implemented load button; made columns have maximum width and wrap words; added header style; fixed default period; fixed some bugs
</commit_message>
<xml_diff>
--- a/orders/order_templates/10.09.2024.xlsx
+++ b/orders/order_templates/10.09.2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\software-purchases\orders\order_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEE9458-4CD4-435C-A3DE-AA837BD57EB2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FCFE1C-66C7-4C26-8CBD-CAF1AF250FB0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="270" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10927,7 +10927,7 @@
   <dimension ref="A1:W449"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>